<commit_message>
Add generated leaderboard data - 03-01-2024 02:16:11
</commit_message>
<xml_diff>
--- a/LeaderboardsStorage/CurrentCodeRankingLeaderboard.xlsx
+++ b/LeaderboardsStorage/CurrentCodeRankingLeaderboard.xlsx
@@ -2675,7 +2675,7 @@
     <t>dhansaib6</t>
   </si>
   <si>
-    <t>33.44%</t>
+    <t>33.48%</t>
   </si>
   <si>
     <t>21r01a04k0</t>
@@ -6305,7 +6305,7 @@
     <t>21r01ajyys</t>
   </si>
   <si>
-    <t>16.55%</t>
+    <t>16.59%</t>
   </si>
   <si>
     <t>21r01a04k1</t>
@@ -20556,7 +20556,7 @@
         <v>10.0</v>
       </c>
       <c r="G201" t="n" s="2">
-        <v>30.0</v>
+        <v>34.0</v>
       </c>
       <c r="H201" t="s" s="2">
         <v>886</v>
@@ -32656,7 +32656,7 @@
         <v>10.0</v>
       </c>
       <c r="G476" t="n" s="2">
-        <v>16.0</v>
+        <v>20.0</v>
       </c>
       <c r="H476" t="s" s="2">
         <v>2094</v>

</xml_diff>